<commit_message>
Update date and prices for BTC and ETH options
</commit_message>
<xml_diff>
--- a/server/data/btc-5am-7am-backtest.xlsx
+++ b/server/data/btc-5am-7am-backtest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codeputs\ongoing\python_trading\crypto_option_deltaexchange\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codeputs\ongoing\crypto_option_deltaexchange\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E746F6-CF2C-4A67-BBFA-E2AF98853EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E649443-07DC-4FA3-A080-FE1CFF7B5CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14762,8 +14762,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M128" sqref="M128"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K128" sqref="K128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14833,7 +14833,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -15097,7 +15097,7 @@
         <v>-89.215686274509807</v>
       </c>
     </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -15295,7 +15295,7 @@
         <v>5.5718475073313778</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -15559,7 +15559,7 @@
         <v>12.76595744680851</v>
       </c>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -15757,7 +15757,7 @@
         <v>-19.631901840490798</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -16021,7 +16021,7 @@
         <v>-9.7597597597597598</v>
       </c>
     </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -16218,7 +16218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -16482,7 +16482,7 @@
         <v>-34.606986899563317</v>
       </c>
     </row>
-    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -16680,7 +16680,7 @@
         <v>-17.3841059602649</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -16944,7 +16944,7 @@
         <v>170.11952191235059</v>
       </c>
     </row>
-    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -17142,7 +17142,7 @@
         <v>263.63636363636363</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -17406,7 +17406,7 @@
         <v>74.074074074074076</v>
       </c>
     </row>
-    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -17603,7 +17603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -17867,7 +17867,7 @@
         <v>-0.89820359281437123</v>
       </c>
     </row>
-    <row r="48" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -18065,7 +18065,7 @@
         <v>-26.7816091954023</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -18328,7 +18328,7 @@
         <v>98.454935622317592</v>
       </c>
     </row>
-    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -18526,7 +18526,7 @@
         <v>-32.79145942011403</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>75</v>
       </c>
@@ -18790,7 +18790,7 @@
         <v>76.630434782608688</v>
       </c>
     </row>
-    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -18988,7 +18988,7 @@
         <v>-9.1254752851711025</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -19251,7 +19251,7 @@
         <v>40.731070496083547</v>
       </c>
     </row>
-    <row r="69" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>86</v>
       </c>
@@ -19449,7 +19449,7 @@
         <v>4.2338709677419351</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>89</v>
       </c>
@@ -19713,7 +19713,7 @@
         <v>96.938775510204081</v>
       </c>
     </row>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>93</v>
       </c>
@@ -19911,7 +19911,7 @@
         <v>-61.013370865587611</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>96</v>
       </c>
@@ -20175,7 +20175,7 @@
         <v>189.31297709923663</v>
       </c>
     </row>
-    <row r="83" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>100</v>
       </c>
@@ -20373,7 +20373,7 @@
         <v>-7.5657894736842106</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>103</v>
       </c>
@@ -20636,7 +20636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>107</v>
       </c>
@@ -20834,7 +20834,7 @@
         <v>89.772727272727266</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>110</v>
       </c>
@@ -21098,7 +21098,7 @@
         <v>223.94366197183101</v>
       </c>
     </row>
-    <row r="97" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -21296,7 +21296,7 @@
         <v>-0.24752475247524752</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -21560,7 +21560,7 @@
         <v>-17.548076923076923</v>
       </c>
     </row>
-    <row r="104" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>121</v>
       </c>
@@ -21758,7 +21758,7 @@
         <v>346.66666666666669</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>124</v>
       </c>
@@ -22022,7 +22022,7 @@
         <v>189.34426229508196</v>
       </c>
     </row>
-    <row r="111" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>128</v>
       </c>
@@ -22220,7 +22220,7 @@
         <v>-28.711985688729875</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>131</v>
       </c>
@@ -22484,7 +22484,7 @@
         <v>77.65432098765433</v>
       </c>
     </row>
-    <row r="118" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>135</v>
       </c>
@@ -22682,7 +22682,7 @@
         <v>462.16216216216219</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>138</v>
       </c>
@@ -23182,7 +23182,7 @@
   <autoFilter ref="A1:U125" xr:uid="{00000000-0001-0000-0200-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Monday"/>
+        <filter val="Friday"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>